<commit_message>
Updated the research timeline to reflect current topics and completion data
</commit_message>
<xml_diff>
--- a/Misc/Research_Timeline.xlsx
+++ b/Misc/Research_Timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whitlock\Desktop\Work\Capstone_2018\CapstoneProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whitlock\Desktop\Work\Capstone_2018\CapstoneProject\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B2CC94D-5C47-46D0-AE4B-21A5914B05D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1C5E286E-2DAC-459E-A6C0-544989819E21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{A9FA6E8A-965F-4ECF-BAC5-3B8369BC2801}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Start Date</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Potential guide for Gantt chart: https://www.officetimeline.com/make-gantt-chart/excel#tutorial-auto</t>
+  </si>
+  <si>
+    <t>Actual Progression</t>
+  </si>
+  <si>
+    <t>Deeper dive into Hadoop components to support Impala</t>
+  </si>
+  <si>
+    <t>* Partially completed, will revisit after file formats</t>
   </si>
 </sst>
 </file>
@@ -99,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,6 +137,18 @@
     <tableColumn id="2" xr3:uid="{6123511B-9F49-4DDB-9B9A-315DE089FE04}" name="End Date"/>
     <tableColumn id="3" xr3:uid="{91491A2A-9B54-4263-9C09-7BE0AA4CFF13}" name=" Description"/>
     <tableColumn id="4" xr3:uid="{75494A5C-0BCF-4FB3-852F-3475EB852BC8}" name="Duration (weeks)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4B703EAE-7B72-4155-956F-1CBF27C2F3BD}" name="Table2" displayName="Table2" ref="H1:J5" totalsRowShown="0">
+  <autoFilter ref="H1:J5" xr:uid="{B20DBA28-6AF0-46A9-BF6B-8229B1FDA2BF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{85B80D97-7069-42C9-B3C1-A7DD738A6B95}" name="Actual Progression"/>
+    <tableColumn id="2" xr3:uid="{B0F0EC7B-DF40-4D90-96C5-AA0E99227C97}" name="Start Date"/>
+    <tableColumn id="3" xr3:uid="{1F202B0D-C35F-43A6-B307-DAA7BE9AE267}" name="End Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -429,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D47787-9B35-4F7E-BC95-106466D21E11}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +463,12 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +481,17 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43435</v>
       </c>
@@ -470,8 +504,14 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>43474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43449</v>
       </c>
@@ -484,8 +524,17 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>43474</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43107</v>
       </c>
@@ -498,8 +547,14 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43132</v>
       </c>
@@ -512,8 +567,14 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2">
+        <v>43485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43138</v>
       </c>
@@ -527,7 +588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43160</v>
       </c>
@@ -541,7 +602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43180</v>
       </c>
@@ -555,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43197</v>
       </c>
@@ -569,15 +630,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated research timeline for next weeks topics
</commit_message>
<xml_diff>
--- a/Misc/Research_Timeline.xlsx
+++ b/Misc/Research_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whitlock\Desktop\Work\Capstone_2018\CapstoneProject\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1C5E286E-2DAC-459E-A6C0-544989819E21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F5DB7F-D0D2-4E02-BF69-C12804A89A42}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{A9FA6E8A-965F-4ECF-BAC5-3B8369BC2801}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Start Date</t>
   </si>
@@ -143,8 +143,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4B703EAE-7B72-4155-956F-1CBF27C2F3BD}" name="Table2" displayName="Table2" ref="H1:J5" totalsRowShown="0">
-  <autoFilter ref="H1:J5" xr:uid="{B20DBA28-6AF0-46A9-BF6B-8229B1FDA2BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4B703EAE-7B72-4155-956F-1CBF27C2F3BD}" name="Table2" displayName="Table2" ref="H1:J7" totalsRowShown="0">
+  <autoFilter ref="H1:J7" xr:uid="{B20DBA28-6AF0-46A9-BF6B-8229B1FDA2BF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{85B80D97-7069-42C9-B3C1-A7DD738A6B95}" name="Actual Progression"/>
     <tableColumn id="2" xr3:uid="{B0F0EC7B-DF40-4D90-96C5-AA0E99227C97}" name="Start Date"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +510,9 @@
       <c r="I2" s="2">
         <v>43474</v>
       </c>
+      <c r="J2" s="2">
+        <v>43493</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -530,6 +533,9 @@
       <c r="I3" s="2">
         <v>43474</v>
       </c>
+      <c r="J3" s="2">
+        <v>43493</v>
+      </c>
       <c r="L3" t="s">
         <v>15</v>
       </c>
@@ -573,6 +579,9 @@
       <c r="I5" s="2">
         <v>43485</v>
       </c>
+      <c r="J5" s="2">
+        <v>43493</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -587,6 +596,13 @@
       <c r="D6">
         <v>3</v>
       </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="2">
+        <v>43493</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -601,6 +617,13 @@
       <c r="D7">
         <v>3</v>
       </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2">
+        <v>43493</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>